<commit_message>
Arreglos en fachadas, criterios, agrego agentes, implementaciones e interfaces de convenio y prestacion, corrigo navegabilidad de costo prestacion a prestacion
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -30,9 +30,6 @@
     <t>Martín</t>
   </si>
   <si>
-    <t>Yo</t>
-  </si>
-  <si>
     <t>Culebra</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>TipoPrestacion</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,16 +508,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -525,13 +525,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -540,13 +540,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -555,45 +555,45 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E8" s="1"/>
     </row>

</xml_diff>

<commit_message>
Proyecto en NetBeans y lista de Clases a implementar
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -30,9 +30,6 @@
     <t>Martín</t>
   </si>
   <si>
-    <t>Culebra</t>
-  </si>
-  <si>
     <t>Cama</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>Gabriel</t>
+  </si>
+  <si>
+    <t>yami</t>
   </si>
 </sst>
 </file>
@@ -131,12 +131,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -166,13 +172,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +484,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,17 +514,17 @@
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -525,13 +532,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -540,13 +547,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -555,45 +562,45 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E8" s="1"/>
     </row>

</xml_diff>

<commit_message>
Marco las clases implementadas en el xls
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -93,7 +93,7 @@
     <t>Gabriel</t>
   </si>
   <si>
-    <t>yami</t>
+    <t>Yami</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,10 +582,10 @@
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Yamila - mi parte
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -484,7 +484,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B8" sqref="B8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,13 +593,13 @@
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="1"/>

</xml_diff>

<commit_message>
más proxys y correciones en diagrama de clase clinica
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Pichón</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Yami</t>
+  </si>
+  <si>
+    <t>Monto?</t>
+  </si>
+  <si>
+    <t>FormaPago?</t>
+  </si>
+  <si>
+    <t>Faltan:</t>
   </si>
 </sst>
 </file>
@@ -185,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -194,6 +203,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H12"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +591,7 @@
       <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="1"/>
@@ -619,7 +629,18 @@
       <c r="E8" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Respuesta en el xls
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Pichón</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Faltan:</t>
+  </si>
+  <si>
+    <t>Me dijeron que no las pusiera, que sólo ibamos a hacer el pago en efectivo</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -204,6 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H13"/>
+  <dimension ref="A2:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,6 +644,11 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Marco los intermediarios IPR en el xls
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Pichón</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Me dijeron que no las pusiera, que sólo ibamos a hacer el pago en efectivo</t>
+  </si>
+  <si>
+    <t>IPR Listo</t>
+  </si>
+  <si>
+    <t>Proxy Listo</t>
   </si>
 </sst>
 </file>
@@ -197,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -208,6 +214,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,14 +517,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H14"/>
+  <dimension ref="A2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
@@ -604,16 +613,16 @@
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -650,6 +659,19 @@
       <c r="B14" s="9" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mas IPRs y correcciones
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Pichón</t>
   </si>
@@ -96,38 +96,29 @@
     <t>Yami</t>
   </si>
   <si>
-    <t>Monto?</t>
-  </si>
-  <si>
-    <t>FormaPago?</t>
-  </si>
-  <si>
-    <t>Faltan:</t>
-  </si>
-  <si>
-    <t>Me dijeron que no las pusiera, que sólo ibamos a hacer el pago en efectivo</t>
-  </si>
-  <si>
     <t>Proxy Listo</t>
   </si>
   <si>
-    <t>Nota:</t>
-  </si>
-  <si>
-    <t>IPR + Proxys Listo</t>
-  </si>
-  <si>
-    <t>Recibo lo necesita para guardar el monto de lo que se paga(tiene el mismo sentido que un detalle), y el tipo debe estar en una tabla aparte, aunque sea 1 solo tipo</t>
-  </si>
-  <si>
-    <t>Ok, las tendrán que hacer los que se llevaron 2 clases nomás =P</t>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Monto</t>
+  </si>
+  <si>
+    <t>FormaPago</t>
+  </si>
+  <si>
+    <t>Leyenda:</t>
+  </si>
+  <si>
+    <t>IPR + Proxy Listo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +151,20 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,20 +217,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,17 +536,17 @@
   <dimension ref="A2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -555,35 +561,35 @@
       <c r="D2" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="12">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -596,12 +602,12 @@
         <v>17</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="G4" s="11" t="s">
-        <v>30</v>
+      <c r="G4" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -616,83 +622,76 @@
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="1"/>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
+      <c r="B14" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="B16" s="8"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
IPRCoseguro, IPREstadoFichaInternacion, IPREstadoFacturaCliente listos !
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -214,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -227,7 +227,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -534,7 +533,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,13 +594,13 @@
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1"/>
@@ -660,13 +659,13 @@
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="1"/>

</xml_diff>

<commit_message>
Responsabilidades en la Carga de base de datos
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Pichón</t>
   </si>
@@ -99,15 +99,6 @@
     <t>Proxy Listo</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Monto</t>
-  </si>
-  <si>
-    <t>FormaPago</t>
-  </si>
-  <si>
     <t>Leyenda:</t>
   </si>
   <si>
@@ -115,13 +106,82 @@
   </si>
   <si>
     <t>PERSISTENCIA</t>
+  </si>
+  <si>
+    <t>carga de datos BD</t>
+  </si>
+  <si>
+    <t>paciente</t>
+  </si>
+  <si>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>costo servicio</t>
+  </si>
+  <si>
+    <t>servicio esp.</t>
+  </si>
+  <si>
+    <t>prestacion</t>
+  </si>
+  <si>
+    <t>costo prestacion</t>
+  </si>
+  <si>
+    <t>ficha</t>
+  </si>
+  <si>
+    <t>detalle ficha</t>
+  </si>
+  <si>
+    <t>cama</t>
+  </si>
+  <si>
+    <t>estado cama</t>
+  </si>
+  <si>
+    <t>habitacion</t>
+  </si>
+  <si>
+    <t>coseguro</t>
+  </si>
+  <si>
+    <t>estado factura</t>
+  </si>
+  <si>
+    <t>Estadoficha</t>
+  </si>
+  <si>
+    <t>factura cliente</t>
+  </si>
+  <si>
+    <t>tipo prestacion</t>
+  </si>
+  <si>
+    <t>recibo</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>tipo habitacion</t>
+  </si>
+  <si>
+    <t>convenio</t>
+  </si>
+  <si>
+    <t>Al menos 5 valores por cada entidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OID de las entidades como las genera Java con el UUID </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,8 +226,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,14 +255,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -210,11 +279,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -227,8 +327,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,15 +649,18 @@
     <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>1</v>
@@ -566,11 +674,14 @@
       <c r="E2" s="9">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -586,29 +697,43 @@
       <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="G4" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -622,8 +747,18 @@
         <v>9</v>
       </c>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -637,8 +772,18 @@
         <v>19</v>
       </c>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -654,8 +799,20 @@
       <c r="E7" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -669,27 +826,54 @@
         <v>12</v>
       </c>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="G8" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G10" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Clases a implementar oids
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Pichón</t>
   </si>
@@ -174,12 +174,6 @@
     <t>Cobro al cliente en efectivo, Calculable para la emicion del recibo</t>
   </si>
   <si>
-    <t>OID de las entidades como las genera Java con el UUID, ejemplo:</t>
-  </si>
-  <si>
-    <t>jhftre42-sge4-7tst-35sg-87hw5e4eiarh</t>
-  </si>
-  <si>
     <t>Al menos 5 valores por cada entidad, de los estados solo los que correspondan</t>
   </si>
   <si>
@@ -199,6 +193,9 @@
   </si>
   <si>
     <t>Completada</t>
+  </si>
+  <si>
+    <t>Utilizar los OID del archivo UUID</t>
   </si>
 </sst>
 </file>
@@ -266,7 +263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +294,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -418,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -426,7 +435,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -435,7 +443,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -444,7 +451,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -461,7 +467,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,19 +795,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -840,16 +852,16 @@
       <c r="E3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="8"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -864,42 +876,42 @@
       <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -915,16 +927,16 @@
         <v>19</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -942,202 +954,200 @@
       <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="34"/>
+      <c r="C10" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="33"/>
+      <c r="D11" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="35"/>
+      <c r="D12" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="32"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="29" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="7"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="36"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="20"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="20"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="20"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="20"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="20"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="18"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="20"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="20"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="18"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="24"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
correccion y base de clases de control de facturar cliente
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -302,7 +302,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,6 +458,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -468,12 +474,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,7 +778,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,13 +892,13 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="39" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="8"/>
@@ -1008,28 +1008,28 @@
       <c r="C10" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="37"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="30"/>
+      <c r="E11" s="36"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="38"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
@@ -1039,15 +1039,15 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="35" t="s">
+      <c r="G14" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="36"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
@@ -1057,13 +1057,13 @@
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="18"/>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="39"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="35"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>

</xml_diff>

<commit_message>
dumps de tipos prestacion y habitacion
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -427,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -464,6 +464,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -473,7 +474,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,7 +779,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,8 +791,8 @@
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -892,13 +893,13 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="36" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="8"/>
@@ -908,9 +909,6 @@
       <c r="G5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -927,16 +925,18 @@
         <v>19</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1008,28 +1008,28 @@
       <c r="C10" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="37"/>
+      <c r="E10" s="38"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="36"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="38"/>
+      <c r="E12" s="39"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">

</xml_diff>

<commit_message>
Algunas tablas llenas (cama, estado_cama, habitacion)
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="15480" windowHeight="7995"/>
@@ -207,8 +207,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,6 +485,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -494,8 +496,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,7 +585,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -620,7 +619,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -796,14 +794,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -816,7 +814,7 @@
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="25" t="s">
         <v>29</v>
       </c>
@@ -834,7 +832,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>1</v>
@@ -861,7 +859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -886,10 +884,10 @@
       <c r="H3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="38"/>
+      <c r="J3" s="39"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -912,10 +910,10 @@
       <c r="H4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="42"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -935,10 +933,10 @@
       <c r="G5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="41"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -968,7 +966,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -984,20 +982,20 @@
       <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="3" t="s">
         <v>40</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
@@ -1024,44 +1022,44 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="12"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="B10" s="24" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="39"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E10" s="41"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="38"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E11" s="40"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="40"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E12" s="42"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="29" t="s">
         <v>50</v>
       </c>
@@ -1079,7 +1077,7 @@
       <c r="I14" s="31"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
         <v>51</v>
@@ -1095,7 +1093,7 @@
       <c r="I15" s="34"/>
       <c r="J15" s="35"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="16"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -1107,7 +1105,7 @@
       <c r="I16" s="15"/>
       <c r="J16" s="18"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="16"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1119,7 +1117,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="18"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="19"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -1131,7 +1129,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="16"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1143,7 +1141,7 @@
       <c r="I19" s="11"/>
       <c r="J19" s="18"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="16"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -1155,7 +1153,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="18"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="16"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1167,7 +1165,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="18"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="20"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -1191,24 +1189,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
IRP que faltaban segun el xls, datos en ficha, detalle
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="15480" windowHeight="7995"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Pichón</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Estadoficha</t>
   </si>
   <si>
-    <t>factura cliente</t>
-  </si>
-  <si>
     <t>tipo prestacion</t>
   </si>
   <si>
@@ -202,13 +199,25 @@
   </si>
   <si>
     <t>Archivo:</t>
+  </si>
+  <si>
+    <t>obra social</t>
+  </si>
+  <si>
+    <t>facturaCliente</t>
+  </si>
+  <si>
+    <t>cristia&amp;cristian.sql</t>
+  </si>
+  <si>
+    <t>gabriel.sql</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,15 +270,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,12 +308,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -446,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -483,8 +479,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -585,6 +579,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -619,6 +614,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -794,14 +790,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -811,10 +807,10 @@
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
     <col min="8" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>29</v>
       </c>
@@ -823,16 +819,16 @@
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
       <c r="F1" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="28"/>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
-      <c r="J1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>1</v>
@@ -859,7 +855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -875,19 +871,23 @@
       <c r="E3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="H3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -901,42 +901,46 @@
         <v>17</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="H4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="I5" s="7"/>
+      <c r="J5" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -950,23 +954,23 @@
         <v>19</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -992,10 +996,13 @@
         <v>40</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>62</v>
+      </c>
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
@@ -1019,81 +1026,81 @@
         <v>43</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="24" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="41"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="E10" s="39"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="40"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="D11" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="38"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="42"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="D12" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="40"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" s="31"/>
       <c r="I14" s="31"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="18"/>
       <c r="F15" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="35"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -1105,7 +1112,7 @@
       <c r="I16" s="15"/>
       <c r="J16" s="18"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1117,7 +1124,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="18"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -1129,7 +1136,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1141,7 +1148,7 @@
       <c r="I19" s="11"/>
       <c r="J19" s="18"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -1153,7 +1160,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="18"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1165,7 +1172,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="18"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -1189,24 +1196,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Insert Convenio, estado_factura_cliente, estado_ficha_internacion y coseguro listos
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -794,7 +794,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,16 +1016,16 @@
         <v>12</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="3" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arreglos en el PIC y quito archivos en desuso
</commit_message>
<xml_diff>
--- a/Proyecto/Clases a implementar.xlsx
+++ b/Proyecto/Clases a implementar.xlsx
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +995,7 @@
       <c r="H7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="3" t="s">
         <v>62</v>
       </c>
       <c r="J7" t="s">

</xml_diff>